<commit_message>
Add empty notes page
</commit_message>
<xml_diff>
--- a/dataSource.xlsx
+++ b/dataSource.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\web-dev\langApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA5329B-F339-4F35-BBBD-133D04FFF507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19BDAA6F-388B-43B1-AB91-83786BF71670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{2A374BEE-E35E-4BFC-8052-9979D044A383}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="713">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="714">
   <si>
     <t>ID</t>
   </si>
@@ -2170,9 +2170,6 @@
   </si>
   <si>
     <t>SOURCE</t>
-  </si>
-  <si>
-    <t>Mistral AI</t>
   </si>
   <si>
     <r>
@@ -2375,6 +2372,176 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> "Nous avons aménagé le grenier pour en faire une chambre d'amis."</t>
+    </r>
+  </si>
+  <si>
+    <t>Mistral</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Les termes "davantage" et "d'avantage" sont souvent confondus, mais ils ont des significations et des usages distincts :
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Davantage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Définition :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Davantage" est un adverbe qui signifie "plus" ou "en plus grande quantité." Il est utilisé pour indiquer une augmentation ou une quantité supplémentaire.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Exemples :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+"Je voudrais davantage de temps pour terminer ce projet."
+"Il a besoin de davantage d'informations pour prendre une décision."
+"Elle aimerait davantage de soutien de la part de ses collègues."
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D'avantage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Définition : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"D'avantage" est une expression qui signifie "de bénéfice" ou "de profit." Elle est utilisée pour parler d'un avantage ou d'un bénéfice.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Exemples :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+"Cette nouvelle technologie n'apporte pas d'avantage par rapport à l'ancienne."
+"Il n'y a pas d'avantage à changer de fournisseur pour le moment."
+"Cette solution présente plusieurs d'avantages par rapport aux autres options."
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Différence clé</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+"Davantage" est utilisé pour indiquer une quantité supplémentaire ou une augmentation.
+"D'avantage" est utilisé pour parler d'un bénéfice ou d'un avantage.</t>
     </r>
   </si>
 </sst>
@@ -5409,10 +5576,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35FA9FEF-8384-4E17-BAAA-162616D8C943}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5443,10 +5610,24 @@
         <v>67</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="D2" t="s">
         <v>712</v>
       </c>
-      <c r="D2" t="s">
-        <v>711</v>
+    </row>
+    <row r="3" spans="1:4" ht="273.60000000000002" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="D3" t="s">
+        <v>712</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add function to create notes and add link on home page
</commit_message>
<xml_diff>
--- a/dataSource.xlsx
+++ b/dataSource.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\web-dev\langApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19BDAA6F-388B-43B1-AB91-83786BF71670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C5FF33-F80A-453C-83B2-69A6022F221E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{2A374BEE-E35E-4BFC-8052-9979D044A383}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="714">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="717">
   <si>
     <t>ID</t>
   </si>
@@ -2170,6 +2170,18 @@
   </si>
   <si>
     <t>SOURCE</t>
+  </si>
+  <si>
+    <t>Mistral</t>
+  </si>
+  <si>
+    <t>KEYWORDS</t>
+  </si>
+  <si>
+    <t>déménager, emménager, aménager</t>
+  </si>
+  <si>
+    <t>davantage, d'avantage</t>
   </si>
   <si>
     <r>
@@ -2185,7 +2197,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Déménager</t>
+      <t>#Déménager#</t>
     </r>
     <r>
       <rPr>
@@ -2207,7 +2219,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Définition : </t>
+      <t xml:space="preserve">#Définition :# </t>
     </r>
     <r>
       <rPr>
@@ -2229,7 +2241,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Exemple :</t>
+      <t xml:space="preserve">#Exemple :# </t>
     </r>
     <r>
       <rPr>
@@ -2251,7 +2263,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Emménager</t>
+      <t>#Emménager#</t>
     </r>
     <r>
       <rPr>
@@ -2273,7 +2285,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Définition :</t>
+      <t>#Définition :#</t>
     </r>
     <r>
       <rPr>
@@ -2295,7 +2307,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Exemple :</t>
+      <t>#Exemple :#</t>
     </r>
     <r>
       <rPr>
@@ -2317,7 +2329,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Aménager</t>
+      <t>#Aménager#</t>
     </r>
     <r>
       <rPr>
@@ -2339,7 +2351,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Définition : </t>
+      <t xml:space="preserve">#Définition :# </t>
     </r>
     <r>
       <rPr>
@@ -2361,7 +2373,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Exemple :</t>
+      <t>#Exemple :#</t>
     </r>
     <r>
       <rPr>
@@ -2373,9 +2385,6 @@
       </rPr>
       <t xml:space="preserve"> "Nous avons aménagé le grenier pour en faire une chambre d'amis."</t>
     </r>
-  </si>
-  <si>
-    <t>Mistral</t>
   </si>
   <si>
     <r>
@@ -2391,7 +2400,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Davantage</t>
+      <t>#Davantage#</t>
     </r>
     <r>
       <rPr>
@@ -2413,7 +2422,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Définition :</t>
+      <t>#Définition :#</t>
     </r>
     <r>
       <rPr>
@@ -2435,7 +2444,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Exemples :</t>
+      <t>#Exemples :#</t>
     </r>
     <r>
       <rPr>
@@ -2460,7 +2469,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>D'avantage</t>
+      <t>#D'avantage#</t>
     </r>
     <r>
       <rPr>
@@ -2482,7 +2491,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Définition : </t>
+      <t xml:space="preserve">#Définition :# </t>
     </r>
     <r>
       <rPr>
@@ -2504,7 +2513,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Exemples :</t>
+      <t>#Exemples :#</t>
     </r>
     <r>
       <rPr>
@@ -2529,7 +2538,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Différence clé</t>
+      <t>#Différence clé#</t>
     </r>
     <r>
       <rPr>
@@ -5576,19 +5585,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35FA9FEF-8384-4E17-BAAA-162616D8C943}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14.33203125" customWidth="1"/>
     <col min="3" max="3" width="141" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5601,8 +5611,11 @@
       <c r="D1" s="2" t="s">
         <v>710</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="216" x14ac:dyDescent="0.3">
+      <c r="E1" s="2" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="216" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5610,13 +5623,16 @@
         <v>67</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="D2" t="s">
         <v>711</v>
       </c>
-      <c r="D2" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="273.60000000000002" x14ac:dyDescent="0.3">
+      <c r="E2" s="1" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5624,10 +5640,13 @@
         <v>67</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>713</v>
+        <v>716</v>
       </c>
       <c r="D3" t="s">
-        <v>712</v>
+        <v>711</v>
+      </c>
+      <c r="E3" t="s">
+        <v>714</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add 7 new sentences
</commit_message>
<xml_diff>
--- a/dataSource.xlsx
+++ b/dataSource.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\web-dev\langApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C5FF33-F80A-453C-83B2-69A6022F221E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F1318A-43EC-478A-9447-D9E10DEDE1C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{2A374BEE-E35E-4BFC-8052-9979D044A383}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2A374BEE-E35E-4BFC-8052-9979D044A383}"/>
   </bookViews>
   <sheets>
     <sheet name="Sentences" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="717">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="766">
   <si>
     <t>ID</t>
   </si>
@@ -2185,7 +2185,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Les termes "déménager," "emménager," et "aménager" sont tous liés à des actions concernant des lieux de résidence ou des espaces, mais ils ont des significations distinctes :
+      <t xml:space="preserve">Les termes "déménager," "emménager," et "aménager" sont tous liés à des actions concernant des lieux de résidence ou des espaces, mais ils ont des significations distinctes.
 </t>
     </r>
     <r>
@@ -2388,7 +2388,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Les termes "davantage" et "d'avantage" sont souvent confondus, mais ils ont des significations et des usages distincts :
+      <t xml:space="preserve">Les termes "davantage" et "d'avantage" sont souvent confondus, mais ils ont des significations et des usages distincts.
 </t>
     </r>
     <r>
@@ -2552,6 +2552,153 @@
 "Davantage" est utilisé pour indiquer une quantité supplémentaire ou une augmentation.
 "D'avantage" est utilisé pour parler d'un bénéfice ou d'un avantage.</t>
     </r>
+  </si>
+  <si>
+    <t>Après avoir déménagé de notre ancienne maison, nous avons emménagé dans un appartement plus spacieux.</t>
+  </si>
+  <si>
+    <t>Avant de déménager, nous devons aménager notre nouvelle maison pour qu'elle soit prête à nous accueillir.</t>
+  </si>
+  <si>
+    <t>Ils vont emménager dans leur nouvelle maison dès qu'ils auront fini d'aménager le salon.</t>
+  </si>
+  <si>
+    <t>Déménager dans une nouvelle ville nous permettra de découvrir davantage de nouvelles cultures et traditions.</t>
+  </si>
+  <si>
+    <t>En emménageant dans ce quartier, nous espérons rencontrer davantage de voisins sympathiques.</t>
+  </si>
+  <si>
+    <t>Il faudrait qu'on se voie davantage car j'y vois beaucoup d'avantages.</t>
+  </si>
+  <si>
+    <t>La situation actuelle présente plus d’inconvénients que d’avantages.</t>
+  </si>
+  <si>
+    <t>After moving out of our old house, we moved into a larger flat.</t>
+  </si>
+  <si>
+    <t>Before moving out, we need to get our new house ready for us.</t>
+  </si>
+  <si>
+    <t>They'll be moving into their new house as soon as they've finished fitting out the living room.</t>
+  </si>
+  <si>
+    <t>Moving to a new city will allow us to discover more about new cultures and traditions.</t>
+  </si>
+  <si>
+    <t>By moving to this area, we hope to meet more friendly neighbours.</t>
+  </si>
+  <si>
+    <t>We need to see more of each other, because I see a lot of advantages in that.</t>
+  </si>
+  <si>
+    <t>The current situation has more disadvantages than advantages.</t>
+  </si>
+  <si>
+    <t>Nachdem wir aus unserem alten Haus ausgezogen sind, sind wir in eine geräumigere Wohnung gezogen.</t>
+  </si>
+  <si>
+    <t>Bevor wir umziehen, müssen wir unser neues Haus einrichten, damit es bereit ist, uns aufzunehmen.</t>
+  </si>
+  <si>
+    <t>Sie werden in ihr neues Haus einziehen, sobald sie das Wohnzimmer eingerichtet haben.</t>
+  </si>
+  <si>
+    <t>Der Umzug in eine neue Stadt ermöglicht es uns, mehr von den neuen Kulturen und Traditionen kennenzulernen.</t>
+  </si>
+  <si>
+    <t>Durch den Umzug in diese Gegend hoffen wir, mehr nette Nachbarn zu treffen.</t>
+  </si>
+  <si>
+    <t>Wir sollten uns mehr treffen, weil ich viele Vorteile darin sehe.</t>
+  </si>
+  <si>
+    <t>Die derzeitige Situation hat mehr Nachteile als Vorteile.</t>
+  </si>
+  <si>
+    <t>Na het verlaten van ons oude huis zijn we verhuisd naar een grotere flat.</t>
+  </si>
+  <si>
+    <t>Voordat we verhuizen, moeten we ons nieuwe huis klaarmaken.</t>
+  </si>
+  <si>
+    <t>Ze verhuizen naar hun nieuwe huis zodra ze klaar zijn met het inrichten van de woonkamer.</t>
+  </si>
+  <si>
+    <t>Door te verhuizen naar een nieuwe stad kunnen we meer te weten komen over nieuwe culturen en tradities.</t>
+  </si>
+  <si>
+    <t>Door naar dit gebied te verhuizen, hopen we meer vriendelijke buren te ontmoeten.</t>
+  </si>
+  <si>
+    <t>We moeten elkaar meer gaan zien, want daar zie ik veel voordelen in.</t>
+  </si>
+  <si>
+    <t>De huidige situatie heeft meer nadelen dan voordelen.</t>
+  </si>
+  <si>
+    <t>Depois de sairmos da nossa antiga casa, mudámo-nos para um apartamento maior.</t>
+  </si>
+  <si>
+    <t>Antes de nos mudarmos, temos de preparar a nossa nova casa para nós.</t>
+  </si>
+  <si>
+    <t>Eles vão mudar-se para a nova casa assim que acabarem de equipar a sala de estar.</t>
+  </si>
+  <si>
+    <t>A mudança para uma nova cidade permitir-nos-á descobrir mais sobre novas culturas e tradições.</t>
+  </si>
+  <si>
+    <t>Ao mudarmo-nos para esta zona, esperamos encontrar mais vizinhos simpáticos.</t>
+  </si>
+  <si>
+    <t>Precisamos de nos ver mais uns aos outros, porque vejo muitas vantagens nisso.</t>
+  </si>
+  <si>
+    <t>A situação atual tem mais desvantagens do que vantagens.</t>
+  </si>
+  <si>
+    <t>Después de mudarnos de nuestra antigua casa, nos mudamos a un piso más grande.</t>
+  </si>
+  <si>
+    <t>Antes de mudarnos, tenemos que preparar nuestra nueva casa.</t>
+  </si>
+  <si>
+    <t>Se mudarán a su nueva casa en cuanto terminen de acondicionar el salón.</t>
+  </si>
+  <si>
+    <t>Mudarnos a una nueva ciudad nos permitirá descubrir nuevas culturas y tradiciones.</t>
+  </si>
+  <si>
+    <t>Al mudarnos a esta zona, esperamos conocer a más vecinos amistosos.</t>
+  </si>
+  <si>
+    <t>Tenemos que vernos más, porque le veo muchas ventajas.</t>
+  </si>
+  <si>
+    <t>La situación actual tiene más desventajas que ventajas.</t>
+  </si>
+  <si>
+    <t>Dopo aver lasciato la nostra vecchia casa, ci siamo trasferiti in un appartamento più grande.</t>
+  </si>
+  <si>
+    <t>Prima di traslocare, dobbiamo preparare la nuova casa per noi.</t>
+  </si>
+  <si>
+    <t>Si trasferiranno nella loro nuova casa non appena avranno finito di sistemare il soggiorno.</t>
+  </si>
+  <si>
+    <t>Trasferirci in una nuova città ci permetterà di scoprire nuove culture e tradizioni.</t>
+  </si>
+  <si>
+    <t>Trasferendoci in questa zona, speriamo di incontrare più vicini amichevoli.</t>
+  </si>
+  <si>
+    <t>Dobbiamo vederci di più, perché vedo molti vantaggi in questo.</t>
+  </si>
+  <si>
+    <t>La situazione attuale presenta più svantaggi che vantaggi.</t>
   </si>
 </sst>
 </file>
@@ -2935,23 +3082,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{999B6F8C-E532-4FCD-AE86-54288602CE8F}">
-  <dimension ref="A1:H101"/>
+  <dimension ref="A1:H108"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="C103" sqref="C103"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="F108" sqref="F108"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="37.5546875" customWidth="1"/>
-    <col min="3" max="3" width="48.88671875" customWidth="1"/>
-    <col min="4" max="4" width="58.109375" customWidth="1"/>
-    <col min="5" max="5" width="38.109375" customWidth="1"/>
-    <col min="7" max="7" width="33.33203125" customWidth="1"/>
-    <col min="8" max="8" width="39.5546875" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" customWidth="1"/>
+    <col min="3" max="3" width="48.85546875" customWidth="1"/>
+    <col min="4" max="4" width="58.140625" customWidth="1"/>
+    <col min="5" max="5" width="38.140625" customWidth="1"/>
+    <col min="6" max="6" width="29.28515625" customWidth="1"/>
+    <col min="7" max="7" width="33.28515625" customWidth="1"/>
+    <col min="8" max="8" width="39.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2977,7 +3125,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3003,7 +3151,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3029,7 +3177,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3055,7 +3203,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3081,7 +3229,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3107,7 +3255,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3133,7 +3281,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3159,7 +3307,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3185,7 +3333,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3211,7 +3359,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3237,7 +3385,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3263,7 +3411,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3289,7 +3437,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3315,7 +3463,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3341,7 +3489,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3367,7 +3515,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3393,7 +3541,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3419,7 +3567,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3445,7 +3593,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3471,7 +3619,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3497,7 +3645,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3523,7 +3671,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3549,7 +3697,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3575,7 +3723,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3601,7 +3749,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3627,7 +3775,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3653,7 +3801,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3679,7 +3827,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3705,7 +3853,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3731,7 +3879,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3757,7 +3905,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3783,7 +3931,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3809,7 +3957,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3835,7 +3983,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3861,7 +4009,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3887,7 +4035,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3913,7 +4061,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3939,7 +4087,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3965,7 +4113,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3991,7 +4139,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -4017,7 +4165,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -4043,7 +4191,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4069,7 +4217,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4095,7 +4243,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4121,7 +4269,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -4147,7 +4295,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4173,7 +4321,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4199,7 +4347,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4225,7 +4373,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4251,7 +4399,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4277,7 +4425,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4303,7 +4451,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4329,7 +4477,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -4355,7 +4503,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4381,7 +4529,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -4407,7 +4555,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -4433,7 +4581,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -4459,7 +4607,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -4485,7 +4633,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -4511,7 +4659,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -4537,7 +4685,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -4563,7 +4711,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -4589,7 +4737,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4615,7 +4763,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4641,7 +4789,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -4667,7 +4815,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -4693,7 +4841,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -4719,7 +4867,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -4745,7 +4893,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4771,7 +4919,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -4797,7 +4945,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -4823,7 +4971,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -4849,7 +4997,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -4875,7 +5023,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -4901,7 +5049,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -4927,7 +5075,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -4953,7 +5101,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -4979,7 +5127,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -5005,7 +5153,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -5031,7 +5179,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -5057,7 +5205,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -5083,7 +5231,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -5109,7 +5257,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -5135,7 +5283,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -5161,7 +5309,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -5187,7 +5335,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -5213,7 +5361,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -5239,7 +5387,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -5265,7 +5413,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -5291,7 +5439,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -5317,7 +5465,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -5343,7 +5491,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -5369,7 +5517,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -5395,7 +5543,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -5421,7 +5569,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -5447,7 +5595,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -5473,7 +5621,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -5499,7 +5647,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -5525,7 +5673,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -5551,7 +5699,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -5575,6 +5723,188 @@
       </c>
       <c r="H101" t="s">
         <v>699</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102" t="s">
+        <v>724</v>
+      </c>
+      <c r="C102" t="s">
+        <v>731</v>
+      </c>
+      <c r="D102" t="s">
+        <v>738</v>
+      </c>
+      <c r="E102" t="s">
+        <v>745</v>
+      </c>
+      <c r="F102" t="s">
+        <v>717</v>
+      </c>
+      <c r="G102" t="s">
+        <v>752</v>
+      </c>
+      <c r="H102" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103" t="s">
+        <v>725</v>
+      </c>
+      <c r="C103" t="s">
+        <v>732</v>
+      </c>
+      <c r="D103" t="s">
+        <v>739</v>
+      </c>
+      <c r="E103" t="s">
+        <v>746</v>
+      </c>
+      <c r="F103" t="s">
+        <v>718</v>
+      </c>
+      <c r="G103" t="s">
+        <v>753</v>
+      </c>
+      <c r="H103" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104" t="s">
+        <v>726</v>
+      </c>
+      <c r="C104" t="s">
+        <v>733</v>
+      </c>
+      <c r="D104" t="s">
+        <v>740</v>
+      </c>
+      <c r="E104" t="s">
+        <v>747</v>
+      </c>
+      <c r="F104" t="s">
+        <v>719</v>
+      </c>
+      <c r="G104" t="s">
+        <v>754</v>
+      </c>
+      <c r="H104" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>104</v>
+      </c>
+      <c r="B105" t="s">
+        <v>727</v>
+      </c>
+      <c r="C105" t="s">
+        <v>734</v>
+      </c>
+      <c r="D105" t="s">
+        <v>741</v>
+      </c>
+      <c r="E105" t="s">
+        <v>748</v>
+      </c>
+      <c r="F105" t="s">
+        <v>720</v>
+      </c>
+      <c r="G105" t="s">
+        <v>755</v>
+      </c>
+      <c r="H105" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>105</v>
+      </c>
+      <c r="B106" t="s">
+        <v>728</v>
+      </c>
+      <c r="C106" t="s">
+        <v>735</v>
+      </c>
+      <c r="D106" t="s">
+        <v>742</v>
+      </c>
+      <c r="E106" t="s">
+        <v>749</v>
+      </c>
+      <c r="F106" t="s">
+        <v>721</v>
+      </c>
+      <c r="G106" t="s">
+        <v>756</v>
+      </c>
+      <c r="H106" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>106</v>
+      </c>
+      <c r="B107" t="s">
+        <v>729</v>
+      </c>
+      <c r="C107" t="s">
+        <v>736</v>
+      </c>
+      <c r="D107" t="s">
+        <v>743</v>
+      </c>
+      <c r="E107" t="s">
+        <v>750</v>
+      </c>
+      <c r="F107" t="s">
+        <v>722</v>
+      </c>
+      <c r="G107" t="s">
+        <v>757</v>
+      </c>
+      <c r="H107" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>107</v>
+      </c>
+      <c r="B108" t="s">
+        <v>730</v>
+      </c>
+      <c r="C108" t="s">
+        <v>737</v>
+      </c>
+      <c r="D108" t="s">
+        <v>744</v>
+      </c>
+      <c r="E108" t="s">
+        <v>751</v>
+      </c>
+      <c r="F108" t="s">
+        <v>723</v>
+      </c>
+      <c r="G108" t="s">
+        <v>758</v>
+      </c>
+      <c r="H108" t="s">
+        <v>765</v>
       </c>
     </row>
   </sheetData>
@@ -5587,18 +5917,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35FA9FEF-8384-4E17-BAAA-162616D8C943}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="141" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5615,7 +5945,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="216" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="225" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5632,7 +5962,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="300" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>

</xml_diff>